<commit_message>
finał 2025.08.25 - raporty xlsx do poprawy
</commit_message>
<xml_diff>
--- a/Wycena/Raporty/Raport dla klienta.xlsx
+++ b/Wycena/Raporty/Raport dla klienta.xlsx
@@ -133,7 +133,7 @@
       <row>1</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -158,7 +158,7 @@
       <row>2</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -183,7 +183,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -208,7 +208,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -233,7 +233,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -258,7 +258,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -283,7 +283,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="7" name="Image 7" descr="Picture"/>
@@ -308,7 +308,7 @@
       <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="8" name="Image 8" descr="Picture"/>
@@ -333,7 +333,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="9" name="Image 9" descr="Picture"/>
@@ -358,7 +358,7 @@
       <row>10</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="10" name="Image 10" descr="Picture"/>
@@ -383,7 +383,7 @@
       <row>11</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="11" name="Image 11" descr="Picture"/>
@@ -408,7 +408,7 @@
       <row>12</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="12" name="Image 12" descr="Picture"/>
@@ -433,7 +433,7 @@
       <row>13</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="13" name="Image 13" descr="Picture"/>
@@ -458,7 +458,7 @@
       <row>14</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="14" name="Image 14" descr="Picture"/>
@@ -483,7 +483,7 @@
       <row>15</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="15" name="Image 15" descr="Picture"/>
@@ -508,7 +508,7 @@
       <row>16</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="16" name="Image 16" descr="Picture"/>
@@ -533,7 +533,7 @@
       <row>17</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="17" name="Image 17" descr="Picture"/>
@@ -558,7 +558,7 @@
       <row>18</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="18" name="Image 18" descr="Picture"/>
@@ -583,7 +583,7 @@
       <row>19</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="19" name="Image 19" descr="Picture"/>
@@ -608,7 +608,7 @@
       <row>20</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="20" name="Image 20" descr="Picture"/>
@@ -633,7 +633,7 @@
       <row>21</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="21" name="Image 21" descr="Picture"/>
@@ -658,7 +658,7 @@
       <row>22</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="22" name="Image 22" descr="Picture"/>
@@ -683,7 +683,7 @@
       <row>23</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="23" name="Image 23" descr="Picture"/>
@@ -708,7 +708,7 @@
       <row>24</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="24" name="Image 24" descr="Picture"/>
@@ -733,7 +733,7 @@
       <row>25</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="25" name="Image 25" descr="Picture"/>
@@ -758,7 +758,7 @@
       <row>26</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="26" name="Image 26" descr="Picture"/>
@@ -783,7 +783,7 @@
       <row>27</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="27" name="Image 27" descr="Picture"/>
@@ -808,7 +808,7 @@
       <row>28</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="28" name="Image 28" descr="Picture"/>
@@ -833,7 +833,7 @@
       <row>29</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="29" name="Image 29" descr="Picture"/>
@@ -858,7 +858,7 @@
       <row>30</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="30" name="Image 30" descr="Picture"/>
@@ -883,7 +883,7 @@
       <row>31</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="31" name="Image 31" descr="Picture"/>
@@ -908,7 +908,7 @@
       <row>32</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="32" name="Image 32" descr="Picture"/>
@@ -933,7 +933,7 @@
       <row>33</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525" cy="9525"/>
+    <ext cx="571500" cy="381000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="33" name="Image 33" descr="Picture"/>

</xml_diff>